<commit_message>
ubah nama sheet doang wkwk
</commit_message>
<xml_diff>
--- a/catatan_oop.xlsx
+++ b/catatan_oop.xlsx
@@ -2,17 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditio Pangestu\Documents\GitHub\Makhluk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry Alvin\Documents\GitHub\Makhluk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Isi Dunia" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -487,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update Mandril dan Beruang
</commit_message>
<xml_diff>
--- a/catatan_oop.xlsx
+++ b/catatan_oop.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry Alvin\Documents\GitHub\Makhluk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali-pc\Documents\GitHub\Makhluk-master\Makhluk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="34">
   <si>
     <t>Burung_unta</t>
   </si>
@@ -123,12 +123,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>harimau</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -478,7 +481,7 @@
   <dimension ref="A2:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +846,7 @@
         <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -858,7 +861,7 @@
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -873,9 +876,6 @@
       </c>
       <c r="D26" t="s">
         <v>12</v>
-      </c>
-      <c r="E26" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -889,9 +889,6 @@
       <c r="D27" t="s">
         <v>24</v>
       </c>
-      <c r="E27" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -923,6 +920,9 @@
       <c r="C30" t="s">
         <v>19</v>
       </c>
+      <c r="D30" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
@@ -931,6 +931,9 @@
       </c>
       <c r="C31" t="s">
         <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gajah, BurungUnta, dan catatan_oop
</commit_message>
<xml_diff>
--- a/catatan_oop.xlsx
+++ b/catatan_oop.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="37">
   <si>
     <t>Burung_unta</t>
   </si>
@@ -113,9 +113,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
     <t>t</t>
   </si>
   <si>
@@ -123,6 +120,21 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>Hewan</t>
   </si>
 </sst>
 </file>
@@ -477,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +525,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -569,7 +581,7 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
@@ -578,7 +590,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="3"/>
     </row>
@@ -591,7 +603,7 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2">
         <v>5</v>
@@ -600,7 +612,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -695,7 +707,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -715,7 +727,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
@@ -739,13 +751,13 @@
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
@@ -765,7 +777,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
@@ -799,6 +811,9 @@
       <c r="D21" t="s">
         <v>28</v>
       </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -828,6 +843,9 @@
       <c r="D23" t="s">
         <v>28</v>
       </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -858,7 +876,7 @@
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -890,7 +908,7 @@
         <v>24</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -910,7 +928,7 @@
         <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -930,7 +948,7 @@
         <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>